<commit_message>
Added deals and task code
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11790" windowHeight="2460"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>FirstNme</t>
   </si>
@@ -59,6 +58,63 @@
   </si>
   <si>
     <t>tester</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>prob</t>
+  </si>
+  <si>
+    <t>riyaz</t>
+  </si>
+  <si>
+    <t>This is a sample test case 1</t>
+  </si>
+  <si>
+    <t>This is a sample test case 2</t>
+  </si>
+  <si>
+    <t>This is a sample test case 3</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>iden</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>mrs.</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>hold</t>
+  </si>
+  <si>
+    <t>function</t>
   </si>
 </sst>
 </file>
@@ -392,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,24 +516,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>